<commit_message>
Fixed excel bug with non-words and updated update times and version numbers from yesterday's push
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -11,6 +11,8 @@
     <sheet name="test2" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="test3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="test4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="test5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="test6" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="186">
   <si>
     <t>Word</t>
   </si>
@@ -552,6 +554,30 @@
   </si>
   <si>
     <t>a thin cylindrical pointed writing implement; a rod of marking substance encased in wood</t>
+  </si>
+  <si>
+    <t>Synset('process.n.06')</t>
+  </si>
+  <si>
+    <t>Synset('phenomenon.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('natural_phenomenon.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('artifact.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('relation.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('part.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('language_unit.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('natural_object.n.01')</t>
   </si>
 </sst>
 </file>
@@ -2097,4 +2123,287 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed xhyper not working properly
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,6 +13,9 @@
     <sheet name="test4" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="test5" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="test6" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="test8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="test9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="test10" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="305">
   <si>
     <t>Word</t>
   </si>
@@ -578,6 +581,363 @@
   </si>
   <si>
     <t>Synset('natural_object.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('cow.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('causal_agent.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('person.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('unwelcome_person.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('unpleasant_person.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('unpleasant_woman.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('cow.n.03')</t>
+  </si>
+  <si>
+    <t>Synset('make.v.03')</t>
+  </si>
+  <si>
+    <t>Synset('arouse.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('stimulate.v.03')</t>
+  </si>
+  <si>
+    <t>Synset('frighten.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('awe.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('overawe.v.01')</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>verb</t>
+  </si>
+  <si>
+    <t>Synset('hello.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('greeting.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('adieu.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('farewell.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('physical_phenomenon.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('energy.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('radiation.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('electromagnetic_radiation.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('actinic_radiation.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('instrumentality.n.03')</t>
+  </si>
+  <si>
+    <t>Synset('device.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('source_of_illumination.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.03')</t>
+  </si>
+  <si>
+    <t>Synset('psychological_feature.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('cognition.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('attitude.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('orientation.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('position.n.03')</t>
+  </si>
+  <si>
+    <t>Synset('luminosity.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('attribute.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('property.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('physical_property.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.05')</t>
+  </si>
+  <si>
+    <t>Synset('location.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('region.n.03')</t>
+  </si>
+  <si>
+    <t>Synset('area.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('scene.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.06')</t>
+  </si>
+  <si>
+    <t>Synset('state.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('condition.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.07')</t>
+  </si>
+  <si>
+    <t>Synset('visual_property.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.08')</t>
+  </si>
+  <si>
+    <t>Synset('friend.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.09')</t>
+  </si>
+  <si>
+    <t>Synset('illumination.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.10')</t>
+  </si>
+  <si>
+    <t>Synset('process.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('higher_cognitive_process.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('knowing.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('understanding.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('insight.n.03')</t>
+  </si>
+  <si>
+    <t>Synset('sparkle.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('quality.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('appearance.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('countenance.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('expression.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.12')</t>
+  </si>
+  <si>
+    <t>Synset('public_knowledge.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('inner_light.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('motivation.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('ethical_motive.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.n.14')</t>
+  </si>
+  <si>
+    <t>Synset('signal.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('visual_signal.n.01')</t>
+  </si>
+  <si>
+    <t>Synset('lighter.n.02')</t>
+  </si>
+  <si>
+    <t>Synset('light.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('change.v.02')</t>
+  </si>
+  <si>
+    <t>Synset('lighten.v.05')</t>
+  </si>
+  <si>
+    <t>Synset('light_up.v.05')</t>
+  </si>
+  <si>
+    <t>Synset('burn.v.05')</t>
+  </si>
+  <si>
+    <t>Synset('ignite.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('alight.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('arrive.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('land.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('fall.v.20')</t>
+  </si>
+  <si>
+    <t>Synset('move.v.02')</t>
+  </si>
+  <si>
+    <t>Synset('change_hands.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('fall.v.21')</t>
+  </si>
+  <si>
+    <t>Synset('unhorse.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('travel.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('descend.v.01')</t>
+  </si>
+  <si>
+    <t>Synset('light.a.01')</t>
+  </si>
+  <si>
+    <t>adjective</t>
+  </si>
+  <si>
+    <t>Synset('light.a.02')</t>
+  </si>
+  <si>
+    <t>Synset('light.a.03')</t>
+  </si>
+  <si>
+    <t>Synset('light.a.04')</t>
+  </si>
+  <si>
+    <t>Synset('light.a.05')</t>
+  </si>
+  <si>
+    <t>Synset('light.a.06')</t>
+  </si>
+  <si>
+    <t>Synset('unaccented.s.02')</t>
+  </si>
+  <si>
+    <t>satellite adjective</t>
+  </si>
+  <si>
+    <t>Synset('light.s.08')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.09')</t>
+  </si>
+  <si>
+    <t>Synset('clean.s.03')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.11')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.12')</t>
+  </si>
+  <si>
+    <t>Synset('light.a.13')</t>
+  </si>
+  <si>
+    <t>Synset('light.a.14')</t>
+  </si>
+  <si>
+    <t>Synset('faint.s.04')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.16')</t>
+  </si>
+  <si>
+    <t>Synset('abstemious.s.02')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.18')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.19')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.20')</t>
+  </si>
+  <si>
+    <t>Synset('idle.s.04')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.22')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.23')</t>
+  </si>
+  <si>
+    <t>Synset('light.s.24')</t>
+  </si>
+  <si>
+    <t>Synset('easy.s.10')</t>
+  </si>
+  <si>
+    <t>Synset('lightly.r.02')</t>
+  </si>
+  <si>
+    <t>adverb</t>
+  </si>
+  <si>
+    <t>Synset used</t>
   </si>
 </sst>
 </file>
@@ -618,7 +978,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -996,6 +1356,1456 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:CY48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:103">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:103">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" t="s">
+        <v>207</v>
+      </c>
+      <c r="K2" t="s">
+        <v>208</v>
+      </c>
+      <c r="L2" t="s">
+        <v>209</v>
+      </c>
+      <c r="M2" t="s">
+        <v>210</v>
+      </c>
+      <c r="N2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:103">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" t="s">
+        <v>212</v>
+      </c>
+      <c r="J3" t="s">
+        <v>213</v>
+      </c>
+      <c r="K3" t="s">
+        <v>214</v>
+      </c>
+      <c r="L3" t="s">
+        <v>211</v>
+      </c>
+      <c r="M3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:103">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G4" t="s">
+        <v>217</v>
+      </c>
+      <c r="H4" t="s">
+        <v>218</v>
+      </c>
+      <c r="I4" t="s">
+        <v>219</v>
+      </c>
+      <c r="J4" t="s">
+        <v>220</v>
+      </c>
+      <c r="K4" t="s">
+        <v>215</v>
+      </c>
+      <c r="L4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:103">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" t="s">
+        <v>224</v>
+      </c>
+      <c r="I5" t="s">
+        <v>221</v>
+      </c>
+      <c r="J5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:103">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H6" t="s">
+        <v>227</v>
+      </c>
+      <c r="I6" t="s">
+        <v>228</v>
+      </c>
+      <c r="J6" t="s">
+        <v>229</v>
+      </c>
+      <c r="K6" t="s">
+        <v>225</v>
+      </c>
+      <c r="L6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:103">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" t="s">
+        <v>232</v>
+      </c>
+      <c r="I7" t="s">
+        <v>230</v>
+      </c>
+      <c r="J7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:103">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>222</v>
+      </c>
+      <c r="G8" t="s">
+        <v>223</v>
+      </c>
+      <c r="H8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I8" t="s">
+        <v>233</v>
+      </c>
+      <c r="J8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:103">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G9" t="s">
+        <v>188</v>
+      </c>
+      <c r="H9" t="s">
+        <v>236</v>
+      </c>
+      <c r="I9" t="s">
+        <v>235</v>
+      </c>
+      <c r="J9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:103">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>222</v>
+      </c>
+      <c r="G10" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" t="s">
+        <v>238</v>
+      </c>
+      <c r="I10" t="s">
+        <v>237</v>
+      </c>
+      <c r="J10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:103">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>216</v>
+      </c>
+      <c r="G11" t="s">
+        <v>217</v>
+      </c>
+      <c r="H11" t="s">
+        <v>240</v>
+      </c>
+      <c r="I11" t="s">
+        <v>241</v>
+      </c>
+      <c r="J11" t="s">
+        <v>242</v>
+      </c>
+      <c r="K11" t="s">
+        <v>243</v>
+      </c>
+      <c r="L11" t="s">
+        <v>244</v>
+      </c>
+      <c r="M11" t="s">
+        <v>239</v>
+      </c>
+      <c r="N11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:103">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>222</v>
+      </c>
+      <c r="G12" t="s">
+        <v>246</v>
+      </c>
+      <c r="H12" t="s">
+        <v>247</v>
+      </c>
+      <c r="I12" t="s">
+        <v>248</v>
+      </c>
+      <c r="J12" t="s">
+        <v>249</v>
+      </c>
+      <c r="K12" t="s">
+        <v>245</v>
+      </c>
+      <c r="L12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:103">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>216</v>
+      </c>
+      <c r="G13" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" t="s">
+        <v>251</v>
+      </c>
+      <c r="I13" t="s">
+        <v>250</v>
+      </c>
+      <c r="J13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:103">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>216</v>
+      </c>
+      <c r="G14" t="s">
+        <v>253</v>
+      </c>
+      <c r="H14" t="s">
+        <v>254</v>
+      </c>
+      <c r="I14" t="s">
+        <v>252</v>
+      </c>
+      <c r="J14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:103">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>256</v>
+      </c>
+      <c r="H15" t="s">
+        <v>257</v>
+      </c>
+      <c r="I15" t="s">
+        <v>255</v>
+      </c>
+      <c r="J15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:103">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>181</v>
+      </c>
+      <c r="I16" t="s">
+        <v>212</v>
+      </c>
+      <c r="J16" t="s">
+        <v>213</v>
+      </c>
+      <c r="K16" t="s">
+        <v>258</v>
+      </c>
+      <c r="L16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:103">
+      <c r="A17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" t="s">
+        <v>260</v>
+      </c>
+      <c r="E17" t="s">
+        <v>261</v>
+      </c>
+      <c r="F17" t="s">
+        <v>259</v>
+      </c>
+      <c r="G17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:103">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s">
+        <v>263</v>
+      </c>
+      <c r="E18" t="s">
+        <v>264</v>
+      </c>
+      <c r="F18" t="s">
+        <v>262</v>
+      </c>
+      <c r="G18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:103">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" t="s">
+        <v>266</v>
+      </c>
+      <c r="E19" t="s">
+        <v>267</v>
+      </c>
+      <c r="F19" t="s">
+        <v>265</v>
+      </c>
+      <c r="G19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:103">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
+        <v>264</v>
+      </c>
+      <c r="C20" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" t="s">
+        <v>263</v>
+      </c>
+      <c r="E20" t="s">
+        <v>264</v>
+      </c>
+      <c r="F20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:103">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D21" t="s">
+        <v>269</v>
+      </c>
+      <c r="E21" t="s">
+        <v>270</v>
+      </c>
+      <c r="F21" t="s">
+        <v>271</v>
+      </c>
+      <c r="G21" t="s">
+        <v>268</v>
+      </c>
+      <c r="H21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:103">
+      <c r="A22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E22" t="s">
+        <v>274</v>
+      </c>
+      <c r="F22" t="s">
+        <v>272</v>
+      </c>
+      <c r="G22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:103">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" t="s">
+        <v>275</v>
+      </c>
+      <c r="C23" t="s">
+        <v>276</v>
+      </c>
+      <c r="D23" t="s">
+        <v>275</v>
+      </c>
+      <c r="E23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:103">
+      <c r="A24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" t="s">
+        <v>277</v>
+      </c>
+      <c r="C24" t="s">
+        <v>276</v>
+      </c>
+      <c r="D24" t="s">
+        <v>277</v>
+      </c>
+      <c r="E24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:103">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>278</v>
+      </c>
+      <c r="C25" t="s">
+        <v>276</v>
+      </c>
+      <c r="D25" t="s">
+        <v>278</v>
+      </c>
+      <c r="E25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:103">
+      <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" t="s">
+        <v>279</v>
+      </c>
+      <c r="C26" t="s">
+        <v>276</v>
+      </c>
+      <c r="D26" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:103">
+      <c r="A27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C27" t="s">
+        <v>276</v>
+      </c>
+      <c r="D27" t="s">
+        <v>280</v>
+      </c>
+      <c r="E27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:103">
+      <c r="A28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" t="s">
+        <v>281</v>
+      </c>
+      <c r="C28" t="s">
+        <v>276</v>
+      </c>
+      <c r="D28" t="s">
+        <v>281</v>
+      </c>
+      <c r="E28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:103">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>282</v>
+      </c>
+      <c r="C29" t="s">
+        <v>283</v>
+      </c>
+      <c r="D29" t="s">
+        <v>282</v>
+      </c>
+      <c r="E29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:103">
+      <c r="A30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" t="s">
+        <v>284</v>
+      </c>
+      <c r="C30" t="s">
+        <v>283</v>
+      </c>
+      <c r="D30" t="s">
+        <v>284</v>
+      </c>
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:103">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" t="s">
+        <v>285</v>
+      </c>
+      <c r="C31" t="s">
+        <v>283</v>
+      </c>
+      <c r="D31" t="s">
+        <v>285</v>
+      </c>
+      <c r="E31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:103">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s">
+        <v>286</v>
+      </c>
+      <c r="C32" t="s">
+        <v>283</v>
+      </c>
+      <c r="D32" t="s">
+        <v>286</v>
+      </c>
+      <c r="E32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:103">
+      <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>287</v>
+      </c>
+      <c r="C33" t="s">
+        <v>283</v>
+      </c>
+      <c r="D33" t="s">
+        <v>287</v>
+      </c>
+      <c r="E33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:103">
+      <c r="A34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B34" t="s">
+        <v>288</v>
+      </c>
+      <c r="C34" t="s">
+        <v>283</v>
+      </c>
+      <c r="D34" t="s">
+        <v>288</v>
+      </c>
+      <c r="E34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:103">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" t="s">
+        <v>289</v>
+      </c>
+      <c r="C35" t="s">
+        <v>276</v>
+      </c>
+      <c r="D35" t="s">
+        <v>289</v>
+      </c>
+      <c r="E35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:103">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" t="s">
+        <v>290</v>
+      </c>
+      <c r="C36" t="s">
+        <v>276</v>
+      </c>
+      <c r="D36" t="s">
+        <v>290</v>
+      </c>
+      <c r="E36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:103">
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" t="s">
+        <v>291</v>
+      </c>
+      <c r="C37" t="s">
+        <v>283</v>
+      </c>
+      <c r="D37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:103">
+      <c r="A38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" t="s">
+        <v>292</v>
+      </c>
+      <c r="C38" t="s">
+        <v>283</v>
+      </c>
+      <c r="D38" t="s">
+        <v>292</v>
+      </c>
+      <c r="E38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:103">
+      <c r="A39" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" t="s">
+        <v>293</v>
+      </c>
+      <c r="C39" t="s">
+        <v>283</v>
+      </c>
+      <c r="D39" t="s">
+        <v>293</v>
+      </c>
+      <c r="E39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:103">
+      <c r="A40" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" t="s">
+        <v>294</v>
+      </c>
+      <c r="C40" t="s">
+        <v>283</v>
+      </c>
+      <c r="D40" t="s">
+        <v>294</v>
+      </c>
+      <c r="E40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:103">
+      <c r="A41" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" t="s">
+        <v>295</v>
+      </c>
+      <c r="C41" t="s">
+        <v>283</v>
+      </c>
+      <c r="D41" t="s">
+        <v>295</v>
+      </c>
+      <c r="E41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:103">
+      <c r="A42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" t="s">
+        <v>296</v>
+      </c>
+      <c r="C42" t="s">
+        <v>283</v>
+      </c>
+      <c r="D42" t="s">
+        <v>296</v>
+      </c>
+      <c r="E42" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:103">
+      <c r="A43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" t="s">
+        <v>297</v>
+      </c>
+      <c r="C43" t="s">
+        <v>283</v>
+      </c>
+      <c r="D43" t="s">
+        <v>297</v>
+      </c>
+      <c r="E43" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:103">
+      <c r="A44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" t="s">
+        <v>298</v>
+      </c>
+      <c r="C44" t="s">
+        <v>283</v>
+      </c>
+      <c r="D44" t="s">
+        <v>298</v>
+      </c>
+      <c r="E44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:103">
+      <c r="A45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" t="s">
+        <v>299</v>
+      </c>
+      <c r="C45" t="s">
+        <v>283</v>
+      </c>
+      <c r="D45" t="s">
+        <v>299</v>
+      </c>
+      <c r="E45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:103">
+      <c r="A46" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" t="s">
+        <v>300</v>
+      </c>
+      <c r="C46" t="s">
+        <v>283</v>
+      </c>
+      <c r="D46" t="s">
+        <v>300</v>
+      </c>
+      <c r="E46" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:103">
+      <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" t="s">
+        <v>301</v>
+      </c>
+      <c r="C47" t="s">
+        <v>283</v>
+      </c>
+      <c r="D47" t="s">
+        <v>301</v>
+      </c>
+      <c r="E47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:103">
+      <c r="A48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" t="s">
+        <v>302</v>
+      </c>
+      <c r="C48" t="s">
+        <v>303</v>
+      </c>
+      <c r="D48" t="s">
+        <v>302</v>
+      </c>
+      <c r="E48" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -2212,13 +4022,222 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="19"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="26"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="33.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z5"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2237,10 +4256,70 @@
       <c r="F1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -2249,18 +4328,60 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M2" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P2" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>133</v>
+      </c>
+      <c r="R2" t="s">
+        <v>134</v>
+      </c>
+      <c r="S2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -2275,132 +4396,1791 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" t="s">
+        <v>128</v>
+      </c>
+      <c r="M3" t="s">
+        <v>186</v>
+      </c>
+      <c r="N3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:CY54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:103">
+      <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:103">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" t="s">
+        <v>125</v>
+      </c>
+      <c r="L2" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N2" t="s">
+        <v>128</v>
+      </c>
+      <c r="O2" t="s">
+        <v>129</v>
+      </c>
+      <c r="P2" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" t="s">
+        <v>133</v>
+      </c>
+      <c r="T2" t="s">
+        <v>134</v>
+      </c>
+      <c r="U2" t="s">
+        <v>135</v>
+      </c>
+      <c r="V2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:103">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" t="s">
+        <v>126</v>
+      </c>
+      <c r="M3" t="s">
+        <v>127</v>
+      </c>
+      <c r="N3" t="s">
+        <v>128</v>
+      </c>
+      <c r="O3" t="s">
+        <v>186</v>
+      </c>
+      <c r="P3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:103">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K4" t="s">
+        <v>192</v>
+      </c>
+      <c r="L4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:103">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" t="s">
+        <v>197</v>
+      </c>
+      <c r="I5" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:103">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="I6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:103">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>182</v>
-      </c>
-      <c r="E6" t="s">
-        <v>183</v>
-      </c>
-      <c r="F6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>204</v>
+      </c>
+      <c r="J7" t="s">
+        <v>203</v>
+      </c>
+      <c r="K7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:103">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J8" t="s">
+        <v>207</v>
+      </c>
+      <c r="K8" t="s">
+        <v>208</v>
+      </c>
+      <c r="L8" t="s">
+        <v>209</v>
+      </c>
+      <c r="M8" t="s">
+        <v>210</v>
+      </c>
+      <c r="N8" t="s">
+        <v>205</v>
+      </c>
+      <c r="O8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:103">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="H9" t="s">
+        <v>181</v>
+      </c>
+      <c r="I9" t="s">
+        <v>212</v>
+      </c>
+      <c r="J9" t="s">
+        <v>213</v>
+      </c>
+      <c r="K9" t="s">
+        <v>214</v>
+      </c>
+      <c r="L9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:103">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>216</v>
+      </c>
+      <c r="G10" t="s">
+        <v>217</v>
+      </c>
+      <c r="H10" t="s">
+        <v>218</v>
+      </c>
+      <c r="I10" t="s">
+        <v>219</v>
+      </c>
+      <c r="J10" t="s">
+        <v>220</v>
+      </c>
+      <c r="K10" t="s">
+        <v>215</v>
+      </c>
+      <c r="L10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:103">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H11" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" t="s">
+        <v>221</v>
+      </c>
+      <c r="J11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:103">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F12" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G12" t="s">
+        <v>226</v>
+      </c>
+      <c r="H12" t="s">
+        <v>227</v>
+      </c>
+      <c r="I12" t="s">
+        <v>228</v>
+      </c>
+      <c r="J12" t="s">
+        <v>229</v>
+      </c>
+      <c r="K12" t="s">
+        <v>225</v>
+      </c>
+      <c r="L12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:103">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>222</v>
+      </c>
+      <c r="G13" t="s">
+        <v>231</v>
+      </c>
+      <c r="H13" t="s">
+        <v>232</v>
+      </c>
+      <c r="I13" t="s">
+        <v>230</v>
+      </c>
+      <c r="J13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:103">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>222</v>
+      </c>
+      <c r="G14" t="s">
+        <v>223</v>
+      </c>
+      <c r="H14" t="s">
+        <v>234</v>
+      </c>
+      <c r="I14" t="s">
+        <v>233</v>
+      </c>
+      <c r="J14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:103">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" t="s">
+        <v>188</v>
+      </c>
+      <c r="H15" t="s">
+        <v>236</v>
+      </c>
+      <c r="I15" t="s">
+        <v>235</v>
+      </c>
+      <c r="J15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:103">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>222</v>
+      </c>
+      <c r="G16" t="s">
+        <v>231</v>
+      </c>
+      <c r="H16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I16" t="s">
+        <v>237</v>
+      </c>
+      <c r="J16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:103">
+      <c r="A17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>216</v>
+      </c>
+      <c r="G17" t="s">
+        <v>217</v>
+      </c>
+      <c r="H17" t="s">
+        <v>240</v>
+      </c>
+      <c r="I17" t="s">
+        <v>241</v>
+      </c>
+      <c r="J17" t="s">
+        <v>242</v>
+      </c>
+      <c r="K17" t="s">
+        <v>243</v>
+      </c>
+      <c r="L17" t="s">
+        <v>244</v>
+      </c>
+      <c r="M17" t="s">
+        <v>239</v>
+      </c>
+      <c r="N17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:103">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>222</v>
+      </c>
+      <c r="G18" t="s">
+        <v>246</v>
+      </c>
+      <c r="H18" t="s">
+        <v>247</v>
+      </c>
+      <c r="I18" t="s">
+        <v>248</v>
+      </c>
+      <c r="J18" t="s">
+        <v>249</v>
+      </c>
+      <c r="K18" t="s">
+        <v>245</v>
+      </c>
+      <c r="L18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:103">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>216</v>
+      </c>
+      <c r="G19" t="s">
+        <v>217</v>
+      </c>
+      <c r="H19" t="s">
+        <v>251</v>
+      </c>
+      <c r="I19" t="s">
+        <v>250</v>
+      </c>
+      <c r="J19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:103">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
+        <v>252</v>
+      </c>
+      <c r="C20" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" t="s">
+        <v>253</v>
+      </c>
+      <c r="H20" t="s">
+        <v>254</v>
+      </c>
+      <c r="I20" t="s">
+        <v>252</v>
+      </c>
+      <c r="J20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:103">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>256</v>
+      </c>
+      <c r="H21" t="s">
+        <v>257</v>
+      </c>
+      <c r="I21" t="s">
+        <v>255</v>
+      </c>
+      <c r="J21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:103">
+      <c r="A22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H22" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" t="s">
-        <v>185</v>
+      <c r="I22" t="s">
+        <v>212</v>
+      </c>
+      <c r="J22" t="s">
+        <v>213</v>
+      </c>
+      <c r="K22" t="s">
+        <v>258</v>
+      </c>
+      <c r="L22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:103">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" t="s">
+        <v>260</v>
+      </c>
+      <c r="E23" t="s">
+        <v>261</v>
+      </c>
+      <c r="F23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:103">
+      <c r="A24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" t="s">
+        <v>262</v>
+      </c>
+      <c r="C24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" t="s">
+        <v>263</v>
+      </c>
+      <c r="E24" t="s">
+        <v>264</v>
+      </c>
+      <c r="F24" t="s">
+        <v>262</v>
+      </c>
+      <c r="G24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:103">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>265</v>
+      </c>
+      <c r="C25" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" t="s">
+        <v>266</v>
+      </c>
+      <c r="E25" t="s">
+        <v>267</v>
+      </c>
+      <c r="F25" t="s">
+        <v>265</v>
+      </c>
+      <c r="G25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:103">
+      <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" t="s">
+        <v>200</v>
+      </c>
+      <c r="D26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E26" t="s">
+        <v>264</v>
+      </c>
+      <c r="F26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:103">
+      <c r="A27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" t="s">
+        <v>268</v>
+      </c>
+      <c r="C27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" t="s">
+        <v>269</v>
+      </c>
+      <c r="E27" t="s">
+        <v>270</v>
+      </c>
+      <c r="F27" t="s">
+        <v>271</v>
+      </c>
+      <c r="G27" t="s">
+        <v>268</v>
+      </c>
+      <c r="H27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:103">
+      <c r="A28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" t="s">
+        <v>272</v>
+      </c>
+      <c r="C28" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" t="s">
+        <v>273</v>
+      </c>
+      <c r="E28" t="s">
+        <v>274</v>
+      </c>
+      <c r="F28" t="s">
+        <v>272</v>
+      </c>
+      <c r="G28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:103">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>275</v>
+      </c>
+      <c r="C29" t="s">
+        <v>276</v>
+      </c>
+      <c r="D29" t="s">
+        <v>275</v>
+      </c>
+      <c r="E29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:103">
+      <c r="A30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" t="s">
+        <v>277</v>
+      </c>
+      <c r="C30" t="s">
+        <v>276</v>
+      </c>
+      <c r="D30" t="s">
+        <v>277</v>
+      </c>
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:103">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" t="s">
+        <v>278</v>
+      </c>
+      <c r="C31" t="s">
+        <v>276</v>
+      </c>
+      <c r="D31" t="s">
+        <v>278</v>
+      </c>
+      <c r="E31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:103">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s">
+        <v>279</v>
+      </c>
+      <c r="C32" t="s">
+        <v>276</v>
+      </c>
+      <c r="D32" t="s">
+        <v>279</v>
+      </c>
+      <c r="E32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:103">
+      <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D33" t="s">
+        <v>280</v>
+      </c>
+      <c r="E33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:103">
+      <c r="A34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B34" t="s">
+        <v>281</v>
+      </c>
+      <c r="C34" t="s">
+        <v>276</v>
+      </c>
+      <c r="D34" t="s">
+        <v>281</v>
+      </c>
+      <c r="E34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:103">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" t="s">
+        <v>282</v>
+      </c>
+      <c r="C35" t="s">
+        <v>283</v>
+      </c>
+      <c r="D35" t="s">
+        <v>282</v>
+      </c>
+      <c r="E35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:103">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" t="s">
+        <v>284</v>
+      </c>
+      <c r="C36" t="s">
+        <v>283</v>
+      </c>
+      <c r="D36" t="s">
+        <v>284</v>
+      </c>
+      <c r="E36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:103">
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" t="s">
+        <v>285</v>
+      </c>
+      <c r="C37" t="s">
+        <v>283</v>
+      </c>
+      <c r="D37" t="s">
+        <v>285</v>
+      </c>
+      <c r="E37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:103">
+      <c r="A38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" t="s">
+        <v>286</v>
+      </c>
+      <c r="C38" t="s">
+        <v>283</v>
+      </c>
+      <c r="D38" t="s">
+        <v>286</v>
+      </c>
+      <c r="E38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:103">
+      <c r="A39" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" t="s">
+        <v>287</v>
+      </c>
+      <c r="C39" t="s">
+        <v>283</v>
+      </c>
+      <c r="D39" t="s">
+        <v>287</v>
+      </c>
+      <c r="E39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:103">
+      <c r="A40" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" t="s">
+        <v>288</v>
+      </c>
+      <c r="C40" t="s">
+        <v>283</v>
+      </c>
+      <c r="D40" t="s">
+        <v>288</v>
+      </c>
+      <c r="E40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:103">
+      <c r="A41" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" t="s">
+        <v>289</v>
+      </c>
+      <c r="C41" t="s">
+        <v>276</v>
+      </c>
+      <c r="D41" t="s">
+        <v>289</v>
+      </c>
+      <c r="E41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:103">
+      <c r="A42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" t="s">
+        <v>290</v>
+      </c>
+      <c r="C42" t="s">
+        <v>276</v>
+      </c>
+      <c r="D42" t="s">
+        <v>290</v>
+      </c>
+      <c r="E42" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:103">
+      <c r="A43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" t="s">
+        <v>291</v>
+      </c>
+      <c r="C43" t="s">
+        <v>283</v>
+      </c>
+      <c r="D43" t="s">
+        <v>291</v>
+      </c>
+      <c r="E43" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:103">
+      <c r="A44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" t="s">
+        <v>292</v>
+      </c>
+      <c r="C44" t="s">
+        <v>283</v>
+      </c>
+      <c r="D44" t="s">
+        <v>292</v>
+      </c>
+      <c r="E44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:103">
+      <c r="A45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" t="s">
+        <v>293</v>
+      </c>
+      <c r="C45" t="s">
+        <v>283</v>
+      </c>
+      <c r="D45" t="s">
+        <v>293</v>
+      </c>
+      <c r="E45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:103">
+      <c r="A46" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" t="s">
+        <v>294</v>
+      </c>
+      <c r="C46" t="s">
+        <v>283</v>
+      </c>
+      <c r="D46" t="s">
+        <v>294</v>
+      </c>
+      <c r="E46" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:103">
+      <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" t="s">
+        <v>295</v>
+      </c>
+      <c r="C47" t="s">
+        <v>283</v>
+      </c>
+      <c r="D47" t="s">
+        <v>295</v>
+      </c>
+      <c r="E47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:103">
+      <c r="A48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" t="s">
+        <v>296</v>
+      </c>
+      <c r="C48" t="s">
+        <v>283</v>
+      </c>
+      <c r="D48" t="s">
+        <v>296</v>
+      </c>
+      <c r="E48" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:103">
+      <c r="A49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" t="s">
+        <v>297</v>
+      </c>
+      <c r="C49" t="s">
+        <v>283</v>
+      </c>
+      <c r="D49" t="s">
+        <v>297</v>
+      </c>
+      <c r="E49" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:103">
+      <c r="A50" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" t="s">
+        <v>298</v>
+      </c>
+      <c r="C50" t="s">
+        <v>283</v>
+      </c>
+      <c r="D50" t="s">
+        <v>298</v>
+      </c>
+      <c r="E50" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:103">
+      <c r="A51" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" t="s">
+        <v>299</v>
+      </c>
+      <c r="C51" t="s">
+        <v>283</v>
+      </c>
+      <c r="D51" t="s">
+        <v>299</v>
+      </c>
+      <c r="E51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:103">
+      <c r="A52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" t="s">
+        <v>300</v>
+      </c>
+      <c r="C52" t="s">
+        <v>283</v>
+      </c>
+      <c r="D52" t="s">
+        <v>300</v>
+      </c>
+      <c r="E52" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:103">
+      <c r="A53" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" t="s">
+        <v>301</v>
+      </c>
+      <c r="C53" t="s">
+        <v>283</v>
+      </c>
+      <c r="D53" t="s">
+        <v>301</v>
+      </c>
+      <c r="E53" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:103">
+      <c r="A54" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" t="s">
+        <v>302</v>
+      </c>
+      <c r="C54" t="s">
+        <v>303</v>
+      </c>
+      <c r="D54" t="s">
+        <v>302</v>
+      </c>
+      <c r="E54" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>